<commit_message>
Slave modbus device ID could be set by modbus register 685
</commit_message>
<xml_diff>
--- a/Docs/T36CTA register list.xlsx
+++ b/Docs/T36CTA register list.xlsx
@@ -465,9 +465,6 @@
     <t>Switch to control RS485 to a master or slave, for reading outdoor light sensor( 1 is master, 0 is slave)</t>
   </si>
   <si>
-    <t>Polling period of master RS485, (1 is 5ms, 200 is 1 second)</t>
-  </si>
-  <si>
     <t>CT Input 5 High Byte</t>
   </si>
   <si>
@@ -804,6 +801,9 @@
       </rPr>
       <t xml:space="preserve"> / Outdoor Lux Low Byte for Type 2</t>
     </r>
+  </si>
+  <si>
+    <t>RS485  slave device modbus ID</t>
   </si>
 </sst>
 </file>
@@ -1246,6 +1246,15 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1271,15 +1280,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1588,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1606,32 +1606,32 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="51" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
@@ -2004,7 +2004,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2015,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2026,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2048,7 +2048,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2059,7 +2059,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2070,7 +2070,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2081,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2092,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2103,7 +2103,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2114,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2125,7 +2125,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2136,7 +2136,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2147,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2158,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2169,7 +2169,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2180,7 +2180,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2191,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2202,7 +2202,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2213,7 +2213,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2224,7 +2224,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2235,7 +2235,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -3195,10 +3195,10 @@
         <v>685</v>
       </c>
       <c r="B153" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3401,233 +3401,233 @@
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="55">
+      <c r="A177" s="45">
         <v>20001</v>
       </c>
-      <c r="B177" s="56">
-        <v>2</v>
-      </c>
-      <c r="C177" s="57" t="s">
+      <c r="B177" s="46">
+        <v>2</v>
+      </c>
+      <c r="C177" s="47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="45">
+        <v>20002</v>
+      </c>
+      <c r="B178" s="46">
+        <v>2</v>
+      </c>
+      <c r="C178" s="47" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="55">
-        <v>20002</v>
-      </c>
-      <c r="B178" s="56">
-        <v>2</v>
-      </c>
-      <c r="C178" s="57" t="s">
+    <row r="179" spans="1:3">
+      <c r="A179" s="45">
+        <v>20003</v>
+      </c>
+      <c r="B179" s="46">
+        <v>2</v>
+      </c>
+      <c r="C179" s="47" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="55">
-        <v>20003</v>
-      </c>
-      <c r="B179" s="56">
-        <v>2</v>
-      </c>
-      <c r="C179" s="57" t="s">
+    <row r="180" spans="1:3">
+      <c r="A180" s="45">
+        <v>20004</v>
+      </c>
+      <c r="B180" s="46">
+        <v>2</v>
+      </c>
+      <c r="C180" s="47" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="55">
-        <v>20004</v>
-      </c>
-      <c r="B180" s="56">
-        <v>2</v>
-      </c>
-      <c r="C180" s="57" t="s">
+    <row r="181" spans="1:3">
+      <c r="A181" s="45">
+        <v>20005</v>
+      </c>
+      <c r="B181" s="46">
+        <v>2</v>
+      </c>
+      <c r="C181" s="47" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="55">
-        <v>20005</v>
-      </c>
-      <c r="B181" s="56">
-        <v>2</v>
-      </c>
-      <c r="C181" s="57" t="s">
+    <row r="182" spans="1:3">
+      <c r="A182" s="45">
+        <v>20006</v>
+      </c>
+      <c r="B182" s="46">
+        <v>2</v>
+      </c>
+      <c r="C182" s="47" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="55">
-        <v>20006</v>
-      </c>
-      <c r="B182" s="56">
-        <v>2</v>
-      </c>
-      <c r="C182" s="57" t="s">
+    <row r="183" spans="1:3">
+      <c r="A183" s="45">
+        <v>20007</v>
+      </c>
+      <c r="B183" s="46">
+        <v>2</v>
+      </c>
+      <c r="C183" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="45">
+        <v>20008</v>
+      </c>
+      <c r="B184" s="46">
+        <v>2</v>
+      </c>
+      <c r="C184" s="47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="45">
+        <v>20009</v>
+      </c>
+      <c r="B185" s="46">
+        <v>2</v>
+      </c>
+      <c r="C185" s="47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="45">
+        <v>20010</v>
+      </c>
+      <c r="B186" s="46">
+        <v>2</v>
+      </c>
+      <c r="C186" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="45">
+        <v>20011</v>
+      </c>
+      <c r="B187" s="46">
+        <v>2</v>
+      </c>
+      <c r="C187" s="47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="45">
+        <v>20012</v>
+      </c>
+      <c r="B188" s="46">
+        <v>2</v>
+      </c>
+      <c r="C188" s="47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="45">
+        <v>20013</v>
+      </c>
+      <c r="B189" s="46">
+        <v>2</v>
+      </c>
+      <c r="C189" s="47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="45">
+        <v>20014</v>
+      </c>
+      <c r="B190" s="46">
+        <v>2</v>
+      </c>
+      <c r="C190" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="45">
+        <v>20015</v>
+      </c>
+      <c r="B191" s="46">
+        <v>2</v>
+      </c>
+      <c r="C191" s="47" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
-      <c r="A183" s="55">
-        <v>20007</v>
-      </c>
-      <c r="B183" s="56">
-        <v>2</v>
-      </c>
-      <c r="C183" s="57" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="55">
-        <v>20008</v>
-      </c>
-      <c r="B184" s="56">
-        <v>2</v>
-      </c>
-      <c r="C184" s="57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="55">
-        <v>20009</v>
-      </c>
-      <c r="B185" s="56">
-        <v>2</v>
-      </c>
-      <c r="C185" s="57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="55">
-        <v>20010</v>
-      </c>
-      <c r="B186" s="56">
-        <v>2</v>
-      </c>
-      <c r="C186" s="57" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="55">
-        <v>20011</v>
-      </c>
-      <c r="B187" s="56">
-        <v>2</v>
-      </c>
-      <c r="C187" s="57" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188" s="55">
-        <v>20012</v>
-      </c>
-      <c r="B188" s="56">
-        <v>2</v>
-      </c>
-      <c r="C188" s="57" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="55">
-        <v>20013</v>
-      </c>
-      <c r="B189" s="56">
-        <v>2</v>
-      </c>
-      <c r="C189" s="57" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="55">
-        <v>20014</v>
-      </c>
-      <c r="B190" s="56">
-        <v>2</v>
-      </c>
-      <c r="C190" s="57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" s="55">
-        <v>20015</v>
-      </c>
-      <c r="B191" s="56">
-        <v>2</v>
-      </c>
-      <c r="C191" s="57" t="s">
+    <row r="192" spans="1:3">
+      <c r="A192" s="45">
+        <v>20016</v>
+      </c>
+      <c r="B192" s="46">
+        <v>2</v>
+      </c>
+      <c r="C192" s="47" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
-      <c r="A192" s="55">
-        <v>20016</v>
-      </c>
-      <c r="B192" s="56">
-        <v>2</v>
-      </c>
-      <c r="C192" s="57" t="s">
+    <row r="193" spans="1:3">
+      <c r="A193" s="45">
+        <v>20017</v>
+      </c>
+      <c r="B193" s="46">
+        <v>2</v>
+      </c>
+      <c r="C193" s="47" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="55">
-        <v>20017</v>
-      </c>
-      <c r="B193" s="56">
-        <v>2</v>
-      </c>
-      <c r="C193" s="57" t="s">
+    <row r="194" spans="1:3">
+      <c r="A194" s="45">
+        <v>20018</v>
+      </c>
+      <c r="B194" s="46">
+        <v>2</v>
+      </c>
+      <c r="C194" s="47" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
-      <c r="A194" s="55">
-        <v>20018</v>
-      </c>
-      <c r="B194" s="56">
-        <v>2</v>
-      </c>
-      <c r="C194" s="57" t="s">
+    <row r="195" spans="1:3">
+      <c r="A195" s="45">
+        <v>20019</v>
+      </c>
+      <c r="B195" s="46">
+        <v>2</v>
+      </c>
+      <c r="C195" s="47" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
-      <c r="A195" s="55">
-        <v>20019</v>
-      </c>
-      <c r="B195" s="56">
-        <v>2</v>
-      </c>
-      <c r="C195" s="57" t="s">
-        <v>179</v>
-      </c>
-    </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="55">
+      <c r="A196" s="45">
         <v>20020</v>
       </c>
-      <c r="B196" s="56">
-        <v>2</v>
-      </c>
-      <c r="C196" s="57" t="s">
+      <c r="B196" s="46">
+        <v>2</v>
+      </c>
+      <c r="C196" s="47" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="55">
+      <c r="A197" s="45">
         <v>20021</v>
       </c>
-      <c r="B197" s="56">
-        <v>2</v>
-      </c>
-      <c r="C197" s="57" t="s">
+      <c r="B197" s="46">
+        <v>2</v>
+      </c>
+      <c r="C197" s="47" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rev 2.20  T36cta. Solved the radio problem
Change SPI2 to simulate spi, for the random frequence value issue.
Reset the register RegPacketConfig2 of RFM module to make sure it go to
RX mode and could receive messages.
</commit_message>
<xml_diff>
--- a/Docs/T36CTA register list.xlsx
+++ b/Docs/T36CTA register list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="182">
   <si>
     <t>Bytes</t>
   </si>
@@ -170,9 +170,6 @@
     <t>RFM69 Module Node ID</t>
   </si>
   <si>
-    <t>RFM69 Module Mode</t>
-  </si>
-  <si>
     <t>RFM69 RegOpMode</t>
   </si>
   <si>
@@ -463,9 +460,6 @@
   </si>
   <si>
     <t>Switch to control RS485 to a master or slave, for reading outdoor light sensor( 1 is master, 0 is slave)</t>
-  </si>
-  <si>
-    <t>Polling period of master RS485, (1 is 5ms, 200 is 1 second)</t>
   </si>
   <si>
     <t>CT Input 5 High Byte</t>
@@ -804,6 +798,18 @@
       </rPr>
       <t xml:space="preserve"> / Outdoor Lux Low Byte for Type 2</t>
     </r>
+  </si>
+  <si>
+    <t>RS485  slave device modbus ID</t>
+  </si>
+  <si>
+    <t>RFM69 Module bitrate</t>
+  </si>
+  <si>
+    <t>RFM69 Module signal strength(RSSI)</t>
+  </si>
+  <si>
+    <t>RFM69 Module Deadmaster Switch (1-enable, 0-disable. default is disable)</t>
   </si>
 </sst>
 </file>
@@ -968,7 +974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1122,6 +1128,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1134,7 +1151,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1246,6 +1263,15 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1272,14 +1298,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1589,7 +1609,7 @@
   <dimension ref="A1:D197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1606,32 +1626,32 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="51" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
@@ -2004,7 +2024,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2015,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2026,7 +2046,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2048,7 +2068,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2059,7 +2079,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2070,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2081,7 +2101,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2092,7 +2112,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2103,7 +2123,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2114,7 +2134,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2125,7 +2145,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2136,7 +2156,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2147,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2158,7 +2178,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2169,7 +2189,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2180,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2191,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2202,7 +2222,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2213,7 +2233,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2224,7 +2244,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2235,7 +2255,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2255,7 +2275,7 @@
       <c r="A64" s="44"/>
       <c r="B64" s="44"/>
       <c r="C64" s="44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2266,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2277,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2288,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2299,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2310,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2321,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2332,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2343,7 +2363,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2354,7 +2374,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2365,7 +2385,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2376,7 +2396,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2387,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2398,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2409,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2420,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2431,7 +2451,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2442,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2453,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2464,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2475,7 +2495,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2486,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2497,7 +2517,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2508,7 +2528,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2519,7 +2539,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2530,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2541,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2552,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2563,7 +2583,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2574,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2585,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2596,7 +2616,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2607,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2618,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2629,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2640,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2651,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2662,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2673,7 +2693,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2684,7 +2704,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2695,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2706,7 +2726,7 @@
         <v>1</v>
       </c>
       <c r="C105" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2717,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="C106" s="43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2728,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="C107" s="43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2739,7 +2759,7 @@
         <v>1</v>
       </c>
       <c r="C108" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2750,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="C109" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2761,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="C110" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2772,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="C111" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2783,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="C112" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2794,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="C113" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2805,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2816,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2827,7 +2847,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2838,7 +2858,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2849,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2860,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2871,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2882,18 +2902,18 @@
         <v>1</v>
       </c>
       <c r="C121" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B122" s="41">
         <v>1</v>
       </c>
       <c r="C122" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2904,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2915,7 +2935,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3057,7 +3077,7 @@
         <v>2</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3090,7 +3110,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3100,19 +3120,31 @@
       <c r="B142" s="20">
         <v>2</v>
       </c>
-      <c r="C142" s="9" t="s">
-        <v>144</v>
+      <c r="C142" s="58" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="13"/>
-      <c r="B143" s="20"/>
-      <c r="C143" s="9"/>
+      <c r="A143" s="13">
+        <v>615</v>
+      </c>
+      <c r="B143" s="20">
+        <v>1</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="13"/>
-      <c r="B144" s="20"/>
-      <c r="C144" s="9"/>
+      <c r="A144" s="13">
+        <v>616</v>
+      </c>
+      <c r="B144" s="20">
+        <v>1</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="14"/>
@@ -3132,7 +3164,7 @@
         <v>2</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3143,7 +3175,7 @@
         <v>2</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3154,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3165,7 +3197,7 @@
         <v>2</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3176,7 +3208,7 @@
         <v>2</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3187,7 +3219,7 @@
         <v>1</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3195,10 +3227,10 @@
         <v>685</v>
       </c>
       <c r="B153" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3219,7 +3251,7 @@
         <v>2</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D156" s="16"/>
     </row>
@@ -3231,7 +3263,7 @@
         <v>2</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D157" s="16"/>
     </row>
@@ -3243,7 +3275,7 @@
         <v>2</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D158" s="16"/>
     </row>
@@ -3255,7 +3287,7 @@
         <v>1</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="160" spans="1:4" s="24" customFormat="1" ht="14.25">
@@ -3266,16 +3298,16 @@
         <v>2</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="161" spans="1:3" s="24" customFormat="1" ht="14.25">
       <c r="A161" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B161" s="22"/>
       <c r="C161" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="162" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3286,18 +3318,18 @@
         <v>2</v>
       </c>
       <c r="C162" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="163" spans="1:3" s="24" customFormat="1" ht="14.25">
       <c r="A163" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B163" s="25">
+        <v>2</v>
+      </c>
+      <c r="C163" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="B163" s="25">
-        <v>2</v>
-      </c>
-      <c r="C163" s="15" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="164" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3306,7 +3338,7 @@
       </c>
       <c r="B164" s="27"/>
       <c r="C164" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="165" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3315,7 +3347,7 @@
       </c>
       <c r="B165" s="27"/>
       <c r="C165" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="166" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3324,7 +3356,7 @@
       </c>
       <c r="B166" s="27"/>
       <c r="C166" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="167" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3333,7 +3365,7 @@
       </c>
       <c r="B167" s="27"/>
       <c r="C167" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="168" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3342,7 +3374,7 @@
       </c>
       <c r="B168" s="30"/>
       <c r="C168" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="169" spans="1:3" s="24" customFormat="1" ht="14.25">
@@ -3352,20 +3384,20 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B170" s="32"/>
       <c r="C170" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B171" s="32"/>
       <c r="C171" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3375,259 +3407,259 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B173" s="34"/>
       <c r="C173" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B174" s="34"/>
       <c r="C174" s="36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B175" s="34"/>
       <c r="C175" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="55">
+      <c r="A177" s="45">
         <v>20001</v>
       </c>
-      <c r="B177" s="56">
-        <v>2</v>
-      </c>
-      <c r="C177" s="57" t="s">
+      <c r="B177" s="46">
+        <v>2</v>
+      </c>
+      <c r="C177" s="47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="45">
+        <v>20002</v>
+      </c>
+      <c r="B178" s="46">
+        <v>2</v>
+      </c>
+      <c r="C178" s="47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="45">
+        <v>20003</v>
+      </c>
+      <c r="B179" s="46">
+        <v>2</v>
+      </c>
+      <c r="C179" s="47" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="55">
-        <v>20002</v>
-      </c>
-      <c r="B178" s="56">
-        <v>2</v>
-      </c>
-      <c r="C178" s="57" t="s">
+    <row r="180" spans="1:3">
+      <c r="A180" s="45">
+        <v>20004</v>
+      </c>
+      <c r="B180" s="46">
+        <v>2</v>
+      </c>
+      <c r="C180" s="47" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="55">
-        <v>20003</v>
-      </c>
-      <c r="B179" s="56">
-        <v>2</v>
-      </c>
-      <c r="C179" s="57" t="s">
+    <row r="181" spans="1:3">
+      <c r="A181" s="45">
+        <v>20005</v>
+      </c>
+      <c r="B181" s="46">
+        <v>2</v>
+      </c>
+      <c r="C181" s="47" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="55">
-        <v>20004</v>
-      </c>
-      <c r="B180" s="56">
-        <v>2</v>
-      </c>
-      <c r="C180" s="57" t="s">
+    <row r="182" spans="1:3">
+      <c r="A182" s="45">
+        <v>20006</v>
+      </c>
+      <c r="B182" s="46">
+        <v>2</v>
+      </c>
+      <c r="C182" s="47" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="55">
-        <v>20005</v>
-      </c>
-      <c r="B181" s="56">
-        <v>2</v>
-      </c>
-      <c r="C181" s="57" t="s">
+    <row r="183" spans="1:3">
+      <c r="A183" s="45">
+        <v>20007</v>
+      </c>
+      <c r="B183" s="46">
+        <v>2</v>
+      </c>
+      <c r="C183" s="47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="45">
+        <v>20008</v>
+      </c>
+      <c r="B184" s="46">
+        <v>2</v>
+      </c>
+      <c r="C184" s="47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="45">
+        <v>20009</v>
+      </c>
+      <c r="B185" s="46">
+        <v>2</v>
+      </c>
+      <c r="C185" s="47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="45">
+        <v>20010</v>
+      </c>
+      <c r="B186" s="46">
+        <v>2</v>
+      </c>
+      <c r="C186" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="45">
+        <v>20011</v>
+      </c>
+      <c r="B187" s="46">
+        <v>2</v>
+      </c>
+      <c r="C187" s="47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="45">
+        <v>20012</v>
+      </c>
+      <c r="B188" s="46">
+        <v>2</v>
+      </c>
+      <c r="C188" s="47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="45">
+        <v>20013</v>
+      </c>
+      <c r="B189" s="46">
+        <v>2</v>
+      </c>
+      <c r="C189" s="47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="45">
+        <v>20014</v>
+      </c>
+      <c r="B190" s="46">
+        <v>2</v>
+      </c>
+      <c r="C190" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="45">
+        <v>20015</v>
+      </c>
+      <c r="B191" s="46">
+        <v>2</v>
+      </c>
+      <c r="C191" s="47" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="55">
-        <v>20006</v>
-      </c>
-      <c r="B182" s="56">
-        <v>2</v>
-      </c>
-      <c r="C182" s="57" t="s">
+    <row r="192" spans="1:3">
+      <c r="A192" s="45">
+        <v>20016</v>
+      </c>
+      <c r="B192" s="46">
+        <v>2</v>
+      </c>
+      <c r="C192" s="47" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
-      <c r="A183" s="55">
-        <v>20007</v>
-      </c>
-      <c r="B183" s="56">
-        <v>2</v>
-      </c>
-      <c r="C183" s="57" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="55">
-        <v>20008</v>
-      </c>
-      <c r="B184" s="56">
-        <v>2</v>
-      </c>
-      <c r="C184" s="57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="55">
-        <v>20009</v>
-      </c>
-      <c r="B185" s="56">
-        <v>2</v>
-      </c>
-      <c r="C185" s="57" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="55">
-        <v>20010</v>
-      </c>
-      <c r="B186" s="56">
-        <v>2</v>
-      </c>
-      <c r="C186" s="57" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="55">
-        <v>20011</v>
-      </c>
-      <c r="B187" s="56">
-        <v>2</v>
-      </c>
-      <c r="C187" s="57" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188" s="55">
-        <v>20012</v>
-      </c>
-      <c r="B188" s="56">
-        <v>2</v>
-      </c>
-      <c r="C188" s="57" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="55">
-        <v>20013</v>
-      </c>
-      <c r="B189" s="56">
-        <v>2</v>
-      </c>
-      <c r="C189" s="57" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="55">
-        <v>20014</v>
-      </c>
-      <c r="B190" s="56">
-        <v>2</v>
-      </c>
-      <c r="C190" s="57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" s="55">
-        <v>20015</v>
-      </c>
-      <c r="B191" s="56">
-        <v>2</v>
-      </c>
-      <c r="C191" s="57" t="s">
+    <row r="193" spans="1:3">
+      <c r="A193" s="45">
+        <v>20017</v>
+      </c>
+      <c r="B193" s="46">
+        <v>2</v>
+      </c>
+      <c r="C193" s="47" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
-      <c r="A192" s="55">
-        <v>20016</v>
-      </c>
-      <c r="B192" s="56">
-        <v>2</v>
-      </c>
-      <c r="C192" s="57" t="s">
+    <row r="194" spans="1:3">
+      <c r="A194" s="45">
+        <v>20018</v>
+      </c>
+      <c r="B194" s="46">
+        <v>2</v>
+      </c>
+      <c r="C194" s="47" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="55">
-        <v>20017</v>
-      </c>
-      <c r="B193" s="56">
-        <v>2</v>
-      </c>
-      <c r="C193" s="57" t="s">
+    <row r="195" spans="1:3">
+      <c r="A195" s="45">
+        <v>20019</v>
+      </c>
+      <c r="B195" s="46">
+        <v>2</v>
+      </c>
+      <c r="C195" s="47" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
-      <c r="A194" s="55">
-        <v>20018</v>
-      </c>
-      <c r="B194" s="56">
-        <v>2</v>
-      </c>
-      <c r="C194" s="57" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195" s="55">
-        <v>20019</v>
-      </c>
-      <c r="B195" s="56">
-        <v>2</v>
-      </c>
-      <c r="C195" s="57" t="s">
-        <v>179</v>
-      </c>
-    </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="55">
+      <c r="A196" s="45">
         <v>20020</v>
       </c>
-      <c r="B196" s="56">
-        <v>2</v>
-      </c>
-      <c r="C196" s="57" t="s">
+      <c r="B196" s="46">
+        <v>2</v>
+      </c>
+      <c r="C196" s="47" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="55">
+      <c r="A197" s="45">
         <v>20021</v>
       </c>
-      <c r="B197" s="56">
-        <v>2</v>
-      </c>
-      <c r="C197" s="57" t="s">
+      <c r="B197" s="46">
+        <v>2</v>
+      </c>
+      <c r="C197" s="47" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New register list for type 3
Added 3 registers of gyroscope
</commit_message>
<xml_diff>
--- a/Docs/T36CTA register list.xlsx
+++ b/Docs/T36CTA register list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="185">
   <si>
     <t>Bytes</t>
   </si>
@@ -810,6 +810,15 @@
   </si>
   <si>
     <t>RFM69 Module Deadmaster Switch (1-enable, 0-disable. default is disable)</t>
+  </si>
+  <si>
+    <t>Gyroscope X-axis value</t>
+  </si>
+  <si>
+    <t>Gyroscope Y-axis value</t>
+  </si>
+  <si>
+    <t>Gyroscope Z-axis value</t>
   </si>
 </sst>
 </file>
@@ -1272,6 +1281,9 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1297,9 +1309,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1606,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1626,32 +1635,32 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="51" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="55"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
@@ -3120,7 +3129,7 @@
       <c r="B142" s="20">
         <v>2</v>
       </c>
-      <c r="C142" s="58" t="s">
+      <c r="C142" s="48" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3234,432 +3243,470 @@
       </c>
     </row>
     <row r="154" spans="1:4">
-      <c r="A154" s="28"/>
-      <c r="B154" s="22"/>
-      <c r="C154" s="15"/>
+      <c r="A154" s="28">
+        <v>686</v>
+      </c>
+      <c r="B154" s="22">
+        <v>2</v>
+      </c>
+      <c r="C154" s="15" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="155" spans="1:4">
-      <c r="A155" s="28"/>
-      <c r="B155" s="22"/>
-      <c r="C155" s="15"/>
+      <c r="A155" s="28">
+        <v>687</v>
+      </c>
+      <c r="B155" s="22">
+        <v>2</v>
+      </c>
+      <c r="C155" s="15" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="28">
+        <v>688</v>
+      </c>
+      <c r="B156" s="22">
+        <v>2</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="28"/>
+      <c r="B157" s="22"/>
+      <c r="C157" s="15"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="28"/>
+      <c r="B158" s="22"/>
+      <c r="C158" s="15"/>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="28"/>
+      <c r="B159" s="22"/>
+      <c r="C159" s="15"/>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="28">
         <v>1002</v>
       </c>
-      <c r="B156" s="22">
-        <v>2</v>
-      </c>
-      <c r="C156" s="15" t="s">
+      <c r="B160" s="22">
+        <v>2</v>
+      </c>
+      <c r="C160" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D156" s="16"/>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="A157" s="28">
+      <c r="D160" s="16"/>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="28">
         <v>1003</v>
       </c>
-      <c r="B157" s="22">
-        <v>2</v>
-      </c>
-      <c r="C157" s="15" t="s">
+      <c r="B161" s="22">
+        <v>2</v>
+      </c>
+      <c r="C161" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D157" s="16"/>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158" s="28">
+      <c r="D161" s="16"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="28">
         <v>1004</v>
       </c>
-      <c r="B158" s="22">
-        <v>2</v>
-      </c>
-      <c r="C158" s="15" t="s">
+      <c r="B162" s="22">
+        <v>2</v>
+      </c>
+      <c r="C162" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D158" s="16"/>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159" s="29">
+      <c r="D162" s="16"/>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="29">
         <v>1005</v>
       </c>
-      <c r="B159" s="22">
-        <v>1</v>
-      </c>
-      <c r="C159" s="15" t="s">
+      <c r="B163" s="22">
+        <v>1</v>
+      </c>
+      <c r="C163" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="160" spans="1:4" s="24" customFormat="1" ht="14.25">
-      <c r="A160" s="29">
+    <row r="164" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A164" s="29">
         <v>1008</v>
       </c>
-      <c r="B160" s="22">
-        <v>2</v>
-      </c>
-      <c r="C160" s="15" t="s">
+      <c r="B164" s="22">
+        <v>2</v>
+      </c>
+      <c r="C164" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="161" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A161" s="29" t="s">
+    <row r="165" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A165" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B161" s="22"/>
-      <c r="C161" s="15" t="s">
+      <c r="B165" s="22"/>
+      <c r="C165" s="15" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A162" s="29">
+    <row r="166" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A166" s="29">
         <v>1029</v>
       </c>
-      <c r="B162" s="25">
-        <v>2</v>
-      </c>
-      <c r="C162" s="26" t="s">
+      <c r="B166" s="25">
+        <v>2</v>
+      </c>
+      <c r="C166" s="26" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A163" s="29" t="s">
+    <row r="167" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A167" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B163" s="25">
-        <v>2</v>
-      </c>
-      <c r="C163" s="15" t="s">
+      <c r="B167" s="25">
+        <v>2</v>
+      </c>
+      <c r="C167" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A164" s="29">
+    <row r="168" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A168" s="29">
         <v>1052</v>
       </c>
-      <c r="B164" s="27"/>
-      <c r="C164" s="15" t="s">
+      <c r="B168" s="27"/>
+      <c r="C168" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="165" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A165" s="29">
+    <row r="169" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A169" s="29">
         <v>1053</v>
       </c>
-      <c r="B165" s="27"/>
-      <c r="C165" s="26" t="s">
+      <c r="B169" s="27"/>
+      <c r="C169" s="26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="166" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A166" s="29">
+    <row r="170" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A170" s="29">
         <v>1054</v>
       </c>
-      <c r="B166" s="27"/>
-      <c r="C166" s="15" t="s">
+      <c r="B170" s="27"/>
+      <c r="C170" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="167" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A167" s="29">
+    <row r="171" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A171" s="29">
         <v>1055</v>
       </c>
-      <c r="B167" s="27"/>
-      <c r="C167" s="15" t="s">
+      <c r="B171" s="27"/>
+      <c r="C171" s="15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A168" s="29">
+    <row r="172" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A172" s="29">
         <v>1056</v>
       </c>
-      <c r="B168" s="30"/>
-      <c r="C168" s="31" t="s">
+      <c r="B172" s="30"/>
+      <c r="C172" s="31" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="24" customFormat="1" ht="14.25">
-      <c r="A169" s="29"/>
-      <c r="B169" s="30"/>
-      <c r="C169" s="31"/>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="37" t="s">
+    <row r="173" spans="1:4" s="24" customFormat="1" ht="14.25">
+      <c r="A173" s="29"/>
+      <c r="B173" s="30"/>
+      <c r="C173" s="31"/>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B170" s="32"/>
-      <c r="C170" s="26" t="s">
+      <c r="B174" s="32"/>
+      <c r="C174" s="26" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="37" t="s">
+    <row r="175" spans="1:4">
+      <c r="A175" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="B171" s="32"/>
-      <c r="C171" s="33" t="s">
+      <c r="B175" s="32"/>
+      <c r="C175" s="33" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
-      <c r="A172" s="38"/>
-      <c r="B172" s="34"/>
-      <c r="C172" s="35"/>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" s="39" t="s">
+    <row r="176" spans="1:4">
+      <c r="A176" s="38"/>
+      <c r="B176" s="34"/>
+      <c r="C176" s="35"/>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="B173" s="34"/>
-      <c r="C173" s="36" t="s">
+      <c r="B177" s="34"/>
+      <c r="C177" s="36" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
-      <c r="A174" s="39" t="s">
+    <row r="178" spans="1:3">
+      <c r="A178" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B174" s="34"/>
-      <c r="C174" s="36" t="s">
+      <c r="B178" s="34"/>
+      <c r="C178" s="36" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="39" t="s">
+    <row r="179" spans="1:3">
+      <c r="A179" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="B175" s="34"/>
-      <c r="C175" s="36" t="s">
+      <c r="B179" s="34"/>
+      <c r="C179" s="36" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="A177" s="45">
-        <v>20001</v>
-      </c>
-      <c r="B177" s="46">
-        <v>2</v>
-      </c>
-      <c r="C177" s="47" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="45">
-        <v>20002</v>
-      </c>
-      <c r="B178" s="46">
-        <v>2</v>
-      </c>
-      <c r="C178" s="47" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="45">
-        <v>20003</v>
-      </c>
-      <c r="B179" s="46">
-        <v>2</v>
-      </c>
-      <c r="C179" s="47" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="45">
-        <v>20004</v>
-      </c>
-      <c r="B180" s="46">
-        <v>2</v>
-      </c>
-      <c r="C180" s="47" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="45">
-        <v>20005</v>
+        <v>20001</v>
       </c>
       <c r="B181" s="46">
         <v>2</v>
       </c>
       <c r="C181" s="47" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="45">
-        <v>20006</v>
+        <v>20002</v>
       </c>
       <c r="B182" s="46">
         <v>2</v>
       </c>
       <c r="C182" s="47" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="45">
-        <v>20007</v>
+        <v>20003</v>
       </c>
       <c r="B183" s="46">
         <v>2</v>
       </c>
       <c r="C183" s="47" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="45">
-        <v>20008</v>
+        <v>20004</v>
       </c>
       <c r="B184" s="46">
         <v>2</v>
       </c>
       <c r="C184" s="47" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="45">
-        <v>20009</v>
+        <v>20005</v>
       </c>
       <c r="B185" s="46">
         <v>2</v>
       </c>
       <c r="C185" s="47" t="s">
-        <v>25</v>
+        <v>171</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="45">
-        <v>20010</v>
+        <v>20006</v>
       </c>
       <c r="B186" s="46">
         <v>2</v>
       </c>
       <c r="C186" s="47" t="s">
-        <v>29</v>
+        <v>172</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="45">
-        <v>20011</v>
+        <v>20007</v>
       </c>
       <c r="B187" s="46">
         <v>2</v>
       </c>
       <c r="C187" s="47" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="45">
-        <v>20012</v>
+        <v>20008</v>
       </c>
       <c r="B188" s="46">
         <v>2</v>
       </c>
       <c r="C188" s="47" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="45">
-        <v>20013</v>
+        <v>20009</v>
       </c>
       <c r="B189" s="46">
         <v>2</v>
       </c>
       <c r="C189" s="47" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="45">
-        <v>20014</v>
+        <v>20010</v>
       </c>
       <c r="B190" s="46">
         <v>2</v>
       </c>
       <c r="C190" s="47" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="45">
-        <v>20015</v>
+        <v>20011</v>
       </c>
       <c r="B191" s="46">
         <v>2</v>
       </c>
       <c r="C191" s="47" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="45">
-        <v>20016</v>
+        <v>20012</v>
       </c>
       <c r="B192" s="46">
         <v>2</v>
       </c>
       <c r="C192" s="47" t="s">
-        <v>174</v>
+        <v>33</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="45">
-        <v>20017</v>
+        <v>20013</v>
       </c>
       <c r="B193" s="46">
         <v>2</v>
       </c>
       <c r="C193" s="47" t="s">
-        <v>175</v>
+        <v>35</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="45">
-        <v>20018</v>
+        <v>20014</v>
       </c>
       <c r="B194" s="46">
         <v>2</v>
       </c>
       <c r="C194" s="47" t="s">
-        <v>176</v>
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="45">
-        <v>20019</v>
+        <v>20015</v>
       </c>
       <c r="B195" s="46">
         <v>2</v>
       </c>
       <c r="C195" s="47" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="45">
-        <v>20020</v>
+        <v>20016</v>
       </c>
       <c r="B196" s="46">
         <v>2</v>
       </c>
       <c r="C196" s="47" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="45">
+        <v>20017</v>
+      </c>
+      <c r="B197" s="46">
+        <v>2</v>
+      </c>
+      <c r="C197" s="47" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="45">
+        <v>20018</v>
+      </c>
+      <c r="B198" s="46">
+        <v>2</v>
+      </c>
+      <c r="C198" s="47" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="45">
+        <v>20019</v>
+      </c>
+      <c r="B199" s="46">
+        <v>2</v>
+      </c>
+      <c r="C199" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="45">
+        <v>20020</v>
+      </c>
+      <c r="B200" s="46">
+        <v>2</v>
+      </c>
+      <c r="C200" s="47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="45">
         <v>20021</v>
       </c>
-      <c r="B197" s="46">
-        <v>2</v>
-      </c>
-      <c r="C197" s="47" t="s">
+      <c r="B201" s="46">
+        <v>2</v>
+      </c>
+      <c r="C201" s="47" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified register list spreadsheet
</commit_message>
<xml_diff>
--- a/Docs/T36CTA register list.xlsx
+++ b/Docs/T36CTA register list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="187">
   <si>
     <t>Bytes</t>
   </si>
@@ -819,6 +819,12 @@
   </si>
   <si>
     <t>Gyroscope Z-axis value</t>
+  </si>
+  <si>
+    <t>689 ~ 698</t>
+  </si>
+  <si>
+    <t>Accelero and Gyroscope chip's configuration registers (CTRL1_XL(10H)-CTRL10_C(19H)) (only for type 3)</t>
   </si>
 </sst>
 </file>
@@ -1617,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3276,9 +3282,15 @@
       </c>
     </row>
     <row r="157" spans="1:4">
-      <c r="A157" s="28"/>
-      <c r="B157" s="22"/>
-      <c r="C157" s="15"/>
+      <c r="A157" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B157" s="22">
+        <v>1</v>
+      </c>
+      <c r="C157" s="15" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="28"/>

</xml_diff>

<commit_message>
Rev27, save setting of gyro chip's registers. and make udp scan command respnse not broadcast
</commit_message>
<xml_diff>
--- a/Docs/T36CTA register list.xlsx
+++ b/Docs/T36CTA register list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="188">
   <si>
     <t>Bytes</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>Accelero and Gyroscope chip's configuration registers (CTRL1_XL(10H)-CTRL10_C(19H)) (only for type 3)</t>
+  </si>
+  <si>
+    <t>Set 1 to reset Acc &amp; Gyro chip's registers to default, and reboot the board</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1627,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3293,9 +3296,15 @@
       </c>
     </row>
     <row r="158" spans="1:4">
-      <c r="A158" s="28"/>
-      <c r="B158" s="22"/>
-      <c r="C158" s="15"/>
+      <c r="A158" s="28">
+        <v>699</v>
+      </c>
+      <c r="B158" s="22">
+        <v>1</v>
+      </c>
+      <c r="C158" s="15" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="28"/>

</xml_diff>